<commit_message>
Updates Time plan and include in document
</commit_message>
<xml_diff>
--- a/docs/Time Plan.xlsx
+++ b/docs/Time Plan.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E95344A-A54F-4D62-842D-C59D0D0F6485}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40712C2-4519-48E1-9430-4CAAF21FFA38}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4260" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -239,7 +239,7 @@
                   <c:v>43507</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43528</c:v>
+                  <c:v>43559</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>43586</c:v>
@@ -301,7 +301,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>85</c:v>
@@ -310,7 +310,7 @@
                   <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
@@ -447,7 +447,7 @@
                       <c:formatCode>m/d/yyyy</c:formatCode>
                       <c:ptCount val="11"/>
                       <c:pt idx="0">
-                        <c:v>43514</c:v>
+                        <c:v>43542</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>43585</c:v>
@@ -456,10 +456,10 @@
                         <c:v>43585</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>43528</c:v>
+                        <c:v>43559</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>43534</c:v>
+                        <c:v>43565</c:v>
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>43616</c:v>
@@ -1470,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,11 +1503,11 @@
         <v>43500</v>
       </c>
       <c r="C2" s="2">
-        <v>43514</v>
+        <v>43542</v>
       </c>
       <c r="D2">
         <f>C2-B2</f>
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1548,11 +1548,11 @@
         <v>43507</v>
       </c>
       <c r="C5" s="2">
-        <v>43528</v>
+        <v>43559</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1560,10 +1560,10 @@
         <v>12</v>
       </c>
       <c r="B6" s="2">
-        <v>43528</v>
+        <v>43559</v>
       </c>
       <c r="C6" s="2">
-        <v>43534</v>
+        <v>43565</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>

</xml_diff>